<commit_message>
Started script for calculating dissolved gas concentration. Most air sample exetainers were entered in wrong row on site-specific spreadsheets and require editing. I worked through a handful but have a long ways to go.
</commit_message>
<xml_diff>
--- a/SuRGE_Sharepoint/data/ADA/CH4_011_Lake Jacksonville/dataSheets/surgeData011.xlsx
+++ b/SuRGE_Sharepoint/data/ADA/CH4_011_Lake Jacksonville/dataSheets/surgeData011.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa.sharepoint.com/sites/SuRGE/Shared Documents/data/ADA/CH4_011_Lake Jacksonville/dataSheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://usepa-my.sharepoint.com/personal/beaulieu_jake_epa_gov/Documents/gitRepository/SuRGE/SuRGE_Sharepoint/data/ADA/CH4_011_Lake Jacksonville/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1433" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E65C21AB-EA8E-417A-B672-5C486416AAD5}"/>
+  <xr:revisionPtr revIDLastSave="1434" documentId="8_{574317AD-36CA-42B2-83FE-C04BF0299D3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93C59194-40D3-4560-9137-9CECEF6A3B4B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2268" yWindow="2268" windowWidth="34560" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -1368,10 +1368,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1672,8 +1668,8 @@
   <dimension ref="A1:BZ18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="AN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="BF5" sqref="BF5"/>
+      <pane xSplit="2" topLeftCell="AV1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="BT7" sqref="BT7:BV7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2169,15 +2165,6 @@
       <c r="BE3">
         <v>13.2</v>
       </c>
-      <c r="BT3" t="s">
-        <v>185</v>
-      </c>
-      <c r="BU3" t="s">
-        <v>186</v>
-      </c>
-      <c r="BV3" t="s">
-        <v>187</v>
-      </c>
       <c r="BW3">
         <v>2.0499999999999998</v>
       </c>
@@ -2557,6 +2544,15 @@
       </c>
       <c r="BE7">
         <v>21.9</v>
+      </c>
+      <c r="BT7" t="s">
+        <v>185</v>
+      </c>
+      <c r="BU7" t="s">
+        <v>186</v>
+      </c>
+      <c r="BV7" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:78" x14ac:dyDescent="0.3">
@@ -4692,20 +4688,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Record xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4">Shared</Record>
@@ -4745,6 +4727,20 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="29f62856-1543-49d4-a736-4569d363f533" ContentTypeId="0x0101" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5219,9 +5215,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5235,15 +5237,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7D26D44A-9508-4707-B138-18882E5BA6FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{845EA28A-135D-4CD8-9991-40FEAFECD172}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="ed970698-2d60-4bab-a048-d9be527522d9"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>